<commit_message>
Updated sources to match MSPM0 SDK 2.00.00.03
Signed-off-by: Franklin Cooper Jr <fcooper@ti.com>
</commit_message>
<xml_diff>
--- a/docs/chinese/middleware/iqmath/benchmarks/iqmath_benchmarks.xlsx
+++ b/docs/chinese/middleware/iqmath/benchmarks/iqmath_benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\gitfolder\msp-sdk\docs\middleware\iqmath\benchmarks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a0272600\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513D2E1B-664B-40FF-9DBE-5DC81D94970C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B5127A-4559-4947-B742-FC71CFEA138C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{5EFBE1B2-BAC2-4D52-900A-B0810AA556C2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{5EFBE1B2-BAC2-4D52-900A-B0810AA556C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
   <si>
     <t>Function Name</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>Benchmark tests performed with a set of dynamic values, 1000 iterations each. IQ value used is 24, tests run in IAR with Medium optimization (default).</t>
+  </si>
+  <si>
+    <t>IAR 9.50.2</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>CCS 12.6.0</t>
+  </si>
+  <si>
+    <t>IQMATH 1.10.00.xx , High speed Opt</t>
+  </si>
+  <si>
+    <t>IQMath 1.00.00.xx, original measurements, IAR 9.20.x</t>
   </si>
 </sst>
 </file>
@@ -114,12 +129,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -134,15 +155,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -452,266 +538,254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE8DEE8-9C5C-474E-98AE-AF71E4A20B91}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
+      <c r="A1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>98</v>
-      </c>
-      <c r="C2">
-        <v>291</v>
-      </c>
-      <c r="D2">
-        <v>1260</v>
-      </c>
-      <c r="E2">
-        <v>292</v>
-      </c>
-      <c r="F2">
-        <v>1223</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D3">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="E3">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F3">
-        <v>1227</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="C4">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+        <v>289</v>
+      </c>
+      <c r="D4">
+        <v>1262</v>
       </c>
       <c r="E4">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
+        <v>291</v>
+      </c>
+      <c r="F4">
+        <v>1227</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>310</v>
+        <v>21</v>
       </c>
       <c r="C5">
-        <v>521</v>
-      </c>
-      <c r="D5">
-        <v>1889</v>
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
       <c r="E5">
-        <v>522</v>
-      </c>
-      <c r="F5">
-        <v>2056</v>
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C6">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D6">
         <v>1889</v>
       </c>
       <c r="E6">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F6">
-        <v>2058</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>264</v>
+        <v>311</v>
       </c>
       <c r="C7">
-        <v>670</v>
+        <v>523</v>
       </c>
       <c r="D7">
-        <v>1404</v>
+        <v>1889</v>
       </c>
       <c r="E7">
-        <v>671</v>
+        <v>525</v>
       </c>
       <c r="F7">
-        <v>1540</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="C8">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="D8">
-        <v>1379</v>
+        <v>1404</v>
       </c>
       <c r="E8">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="F8">
-        <v>1537</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>105</v>
+        <v>279</v>
       </c>
       <c r="C9">
-        <v>564</v>
+        <v>675</v>
       </c>
       <c r="D9">
-        <v>238</v>
+        <v>1379</v>
       </c>
       <c r="E9">
-        <v>566</v>
+        <v>675</v>
       </c>
       <c r="F9">
-        <v>254</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>638</v>
+        <v>105</v>
       </c>
       <c r="C10">
-        <v>645</v>
+        <v>564</v>
       </c>
       <c r="D10">
-        <v>1663</v>
+        <v>238</v>
       </c>
       <c r="E10">
-        <v>646</v>
+        <v>566</v>
       </c>
       <c r="F10">
-        <v>1694</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>892</v>
+        <v>638</v>
       </c>
       <c r="C11">
-        <v>898</v>
+        <v>645</v>
       </c>
       <c r="D11">
-        <v>1479</v>
+        <v>1663</v>
       </c>
       <c r="E11">
-        <v>905</v>
+        <v>646</v>
       </c>
       <c r="F11">
-        <v>1513</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>892</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>898</v>
       </c>
       <c r="D12">
-        <v>73</v>
+        <v>1479</v>
       </c>
       <c r="E12">
-        <v>11</v>
+        <v>905</v>
       </c>
       <c r="F12">
-        <v>71</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>9</v>
@@ -720,64 +794,1000 @@
         <v>9</v>
       </c>
       <c r="D13">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F13">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="D14">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E14">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>76</v>
+      </c>
+      <c r="E15">
+        <v>65</v>
+      </c>
+      <c r="F15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>52</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>442</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>228</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>443</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>294</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>99</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:C34" si="0">B3-B21</f>
+        <v>-1</v>
+      </c>
+      <c r="D21">
+        <v>293</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E34" si="1">C3-D21</f>
+        <v>-2</v>
+      </c>
+      <c r="F21">
+        <v>1254</v>
+      </c>
+      <c r="G21">
+        <f>D3-F21</f>
+        <v>6</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>98</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>293</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="F22">
+        <v>1258</v>
+      </c>
+      <c r="G22">
+        <f>D4-F22</f>
+        <v>4</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>318</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="D24">
+        <v>524</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="F24">
+        <v>1873</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G34" si="2">D6-F24</f>
+        <v>16</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>319</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="D25">
+        <v>525</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="F25">
+        <v>1883</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>190</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="D26">
+        <v>671</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="F26">
+        <v>1401</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>188</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="D27">
+        <v>678</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="F27">
+        <v>1378</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>109</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="D28">
+        <v>553</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>236</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>605</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D29">
+        <v>604</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="F29">
+        <v>1661</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>828</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="D30">
+        <v>826</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="F30">
+        <v>1472</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>72</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>9</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>69</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>54</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F33">
+        <v>75</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34">
+        <v>51</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>444</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="F34">
+        <v>227</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>607</v>
+      </c>
+      <c r="C38">
+        <f>B3-B38</f>
+        <v>-509</v>
+      </c>
+      <c r="D38">
+        <v>898</v>
+      </c>
+      <c r="E38">
+        <f>C3-D38</f>
+        <v>-607</v>
+      </c>
+      <c r="F38">
+        <v>3421</v>
+      </c>
+      <c r="G38">
+        <f>D3-F38</f>
+        <v>-2161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>607</v>
+      </c>
+      <c r="C39">
+        <f t="shared" ref="C39:C51" si="3">B4-B39</f>
+        <v>-508</v>
+      </c>
+      <c r="D39">
+        <v>884</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39:E51" si="4">C4-D39</f>
+        <v>-595</v>
+      </c>
+      <c r="F39">
+        <v>3448</v>
+      </c>
+      <c r="G39">
+        <f>D4-F39</f>
+        <v>-2186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>53</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="3"/>
+        <v>-32</v>
+      </c>
+      <c r="D40">
+        <v>52</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="4"/>
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>809</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="3"/>
+        <v>-499</v>
+      </c>
+      <c r="D41">
+        <v>1422</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="4"/>
+        <v>-901</v>
+      </c>
+      <c r="F41">
+        <v>3061</v>
+      </c>
+      <c r="G41">
+        <f t="shared" ref="G41:G51" si="5">D6-F41</f>
+        <v>-1172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>810</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="3"/>
+        <v>-499</v>
+      </c>
+      <c r="D42">
+        <v>1424</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="4"/>
+        <v>-901</v>
+      </c>
+      <c r="F42">
+        <v>2613</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="5"/>
+        <v>-724</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>496</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="3"/>
+        <v>-232</v>
+      </c>
+      <c r="D43">
+        <v>1913</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="4"/>
+        <v>-1243</v>
+      </c>
+      <c r="F43">
+        <v>2256</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="5"/>
+        <v>-852</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>496</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="3"/>
+        <v>-217</v>
+      </c>
+      <c r="D44">
+        <v>1968</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="4"/>
+        <v>-1293</v>
+      </c>
+      <c r="F44">
+        <v>2546</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="5"/>
+        <v>-1167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>278</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="3"/>
+        <v>-173</v>
+      </c>
+      <c r="D45">
+        <v>1675</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="4"/>
+        <v>-1111</v>
+      </c>
+      <c r="F45">
+        <v>504</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="5"/>
+        <v>-266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>1748</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="3"/>
+        <v>-1110</v>
+      </c>
+      <c r="D46">
+        <v>1748</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="4"/>
+        <v>-1103</v>
+      </c>
+      <c r="F46">
+        <v>2531</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="5"/>
+        <v>-868</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>2436</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="3"/>
+        <v>-1544</v>
+      </c>
+      <c r="D47">
+        <v>2444</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="4"/>
+        <v>-1546</v>
+      </c>
+      <c r="F47">
+        <v>2710</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="5"/>
+        <v>-1231</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50">
+        <v>74</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="3"/>
+        <v>-40</v>
+      </c>
+      <c r="D50">
+        <v>180</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="4"/>
+        <v>-117</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51">
+        <v>87</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="3"/>
+        <v>-35</v>
+      </c>
+      <c r="D51">
+        <v>1306</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="4"/>
+        <v>-864</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="5"/>
+        <v>226</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C21:C34 G21:G34 E21:E34">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C51 E38:E51 G38:G51">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M21:M34 K21:K34 O21:O34">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>